<commit_message>
pre-2019 pit and schedule mods
</commit_message>
<xml_diff>
--- a/Prime Rib Shopping.xlsx
+++ b/Prime Rib Shopping.xlsx
@@ -8,28 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Office Documents\Recipes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD65487C-04EC-43BC-9B00-E958868A7D84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769F71AB-FB20-4484-A5CC-ECEA5879492B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="540" windowWidth="24870" windowHeight="14775" xr2:uid="{E507F307-8855-40C7-ABAE-3141DD388CDB}"/>
+    <workbookView xWindow="2415" yWindow="705" windowWidth="24870" windowHeight="14775" xr2:uid="{E507F307-8855-40C7-ABAE-3141DD388CDB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Shopping List" sheetId="1" r:id="rId1"/>
+    <sheet name="Schedule" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$3:$E$51</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$3:$E$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Shopping List'!$B$3:$E$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Shopping List'!$A$3:$E$57</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="99">
   <si>
     <t>Ingredient</t>
   </si>
@@ -212,6 +219,120 @@
   </si>
   <si>
     <t>Updated 12/20/2019</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Diner Served</t>
+  </si>
+  <si>
+    <t>Roast Hour 1 (60)</t>
+  </si>
+  <si>
+    <t>Roast Hour 2 (60)</t>
+  </si>
+  <si>
+    <t>Roast Hour 3 (60)</t>
+  </si>
+  <si>
+    <t>WSM Preheat to 250°F (60)</t>
+  </si>
+  <si>
+    <t>Roast Hour 4 (60)</t>
+  </si>
+  <si>
+    <t>Prepare Au Jus (15)</t>
+  </si>
+  <si>
+    <t>Carve Prime Rib (15)</t>
+  </si>
+  <si>
+    <t>Minion Chimney (20)</t>
+  </si>
+  <si>
+    <t>Chimney (30)</t>
+  </si>
+  <si>
+    <t>WK Preheat to 450°F /2nd Chimney (45)</t>
+  </si>
+  <si>
+    <t>Prepare Gravy (15)</t>
+  </si>
+  <si>
+    <t>Carve Turkey (15)</t>
+  </si>
+  <si>
+    <t>Prepare Mashed Potatoes (90)</t>
+  </si>
+  <si>
+    <t>Prepare Brussels Sprouts (30)</t>
+  </si>
+  <si>
+    <t>Roast Brussels Sprouts (45)</t>
+  </si>
+  <si>
+    <t>Dinner Served</t>
+  </si>
+  <si>
+    <t>Turkey Finish begin at 110°F (30)</t>
+  </si>
+  <si>
+    <t>Side Prep</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>Appetizer Prep (15)</t>
+  </si>
+  <si>
+    <t>Guests Arrive</t>
+  </si>
+  <si>
+    <t>Trim Prime Rib, tie, rub, tray (30)</t>
+  </si>
+  <si>
+    <t>Wash Turkey, Season, tray (30)</t>
+  </si>
+  <si>
+    <t>Christmas Morning Casserole (30)</t>
+  </si>
+  <si>
+    <t>Reverse Sear at 122°F (WK) (20)</t>
+  </si>
+  <si>
+    <t>Roast Finish, begin at 117°F, Chimney Start (30)</t>
+  </si>
+  <si>
+    <t>Pull at 158°F</t>
+  </si>
+  <si>
+    <t>Preheat Oven to 400°F (15)</t>
+  </si>
+  <si>
+    <t>White Bread</t>
+  </si>
+  <si>
+    <t>1 lb sausage</t>
+  </si>
+  <si>
+    <t>2 C Shredded Cheddar</t>
+  </si>
+  <si>
+    <t>3 Cups Whole Milk</t>
+  </si>
+  <si>
+    <t>6 Eggs</t>
+  </si>
+  <si>
+    <t>3/4 T dry mustard</t>
+  </si>
+  <si>
+    <t>1 can Cream of Mushroom Soup</t>
+  </si>
+  <si>
+    <t>Breakfast Casserole</t>
   </si>
 </sst>
 </file>
@@ -235,7 +356,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,8 +405,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -308,11 +459,122 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -345,6 +607,84 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -664,10 +1004,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:E57"/>
+  <dimension ref="A2:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,6 +1670,85 @@
       <c r="D57" s="11"/>
       <c r="E57" s="11"/>
     </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="C58" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D58" s="37"/>
+      <c r="E58" s="37"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C59" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C60" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D60" s="37"/>
+      <c r="E60" s="37"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C63" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D63" s="37"/>
+      <c r="E63" s="37"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C64" s="37" t="s">
+        <v>98</v>
+      </c>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
+    </row>
   </sheetData>
   <autoFilter ref="B3:E51" xr:uid="{4B5DFD91-B9A9-43B2-B765-E7256B02CD9E}"/>
   <sortState ref="B4:E57">
@@ -1338,4 +1757,335 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="85" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{864D93B2-6A05-4217-8083-D1FFAA465936}">
+  <dimension ref="A1:E37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:5" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="35">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="35">
+        <v>0.42708333333333298</v>
+      </c>
+      <c r="B4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="35">
+        <v>0.4375</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="35">
+        <v>0.44791666666666602</v>
+      </c>
+      <c r="C6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="36">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="36">
+        <v>0.46875</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="35">
+        <v>0.47916666666666602</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="35">
+        <v>0.48958333333333298</v>
+      </c>
+      <c r="C10" s="16"/>
+      <c r="D10" s="34"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="15"/>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="36">
+        <v>0.51041666666666596</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="35">
+        <v>0.52083333333333304</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="16"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="35">
+        <v>0.531249999999999</v>
+      </c>
+      <c r="B14" s="22"/>
+      <c r="C14" s="16"/>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="35">
+        <v>0.54166666666666596</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="15"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="35">
+        <v>0.55208333333333304</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="35">
+        <v>0.562499999999999</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="16"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="35">
+        <v>0.57291666666666596</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="16"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="36">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="36">
+        <v>0.593749999999999</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="30"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="36">
+        <v>0.60416666666666596</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="36">
+        <v>0.61458333333333304</v>
+      </c>
+      <c r="C22" s="16"/>
+      <c r="D22" s="31"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="36">
+        <v>0.624999999999999</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="30"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="36">
+        <v>0.63541666666666596</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="35">
+        <v>0.64583333333333204</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="35">
+        <v>0.656249999999999</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="35">
+        <v>0.66666666666666596</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="36">
+        <v>0.67708333333333204</v>
+      </c>
+      <c r="C28" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="36">
+        <v>0.687499999999999</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="36">
+        <v>0.69791666666666596</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="35">
+        <v>0.70833333333333204</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="35">
+        <v>0.718749999999999</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="35">
+        <v>0.72916666666666496</v>
+      </c>
+      <c r="B33" s="16"/>
+      <c r="D33" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="35">
+        <v>0.73958333333333204</v>
+      </c>
+      <c r="B34" s="15"/>
+      <c r="C34" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="25">
+        <v>0.749999999999999</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="25">
+        <v>0.76041666666666496</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="25">
+        <v>0.77083333333333204</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>